<commit_message>
docs: added results and further documentation and links
</commit_message>
<xml_diff>
--- a/n_vs_t_table.xlsx
+++ b/n_vs_t_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aronr\Desktop\Desktop\UP_2022-2023\CMSC 180 - T3L\Exercises\180-lab-wk5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52BFDE5B-B3C8-4CA8-ABD6-40DA77FFBE67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A69366D7-4D4C-43B4-90A2-8504123053F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="450" windowWidth="28800" windowHeight="15750" xr2:uid="{FE70C4E7-F22F-443D-A91A-558168A21874}"/>
   </bookViews>
@@ -1180,8 +1180,8 @@
       <xdr:rowOff>4760</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>552450</xdr:colOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>400050</xdr:colOff>
       <xdr:row>33</xdr:row>
       <xdr:rowOff>171449</xdr:rowOff>
     </xdr:to>
@@ -1511,7 +1511,7 @@
   <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U20" sqref="U20"/>
+      <selection activeCell="U15" sqref="U15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>